<commit_message>
Überarbeitung Datenmodel und anmeldung
</commit_message>
<xml_diff>
--- a/testdaten/Firma1/Wahlvorstand_120_Personen.xlsx
+++ b/testdaten/Firma1/Wahlvorstand_120_Personen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_d12\MitbestimmIT\testdaten\Firma1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5119EC47-09A8-4511-8DAF-7ABBCA8FD6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0D7389-FF39-4945-B765-0A6BCE8796A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8430" yWindow="4020" windowWidth="38700" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Personalnummer</t>
   </si>
@@ -94,13 +94,22 @@
   </si>
   <si>
     <t>eMail</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Beerdigungen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +124,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,13 +178,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,7 +395,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -402,92 +427,109 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>105060</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>815</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>105118</v>
+        <v>105060</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>105119</v>
+        <v>105118</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>105120</v>
+        <v>105119</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>105120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>105121</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -507,7 +549,7 @@
     <row r="24" x14ac:dyDescent="0.25"/>
     <row r="25" x14ac:dyDescent="0.25"/>
     <row r="26" x14ac:dyDescent="0.25"/>
-    <row r="1048482" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
     <row r="1048483" x14ac:dyDescent="0.25"/>
     <row r="1048484" x14ac:dyDescent="0.25"/>
     <row r="1048485" x14ac:dyDescent="0.25"/>
@@ -604,6 +646,6 @@
     <row r="1048576" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>